<commit_message>
Updated AtomTypes in the Coarse Grained schema and Excel template.
</commit_message>
<xml_diff>
--- a/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
+++ b/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" firstSheet="13" activeTab="20"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" firstSheet="14" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -32,8 +32,8 @@
     <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId18"/>
     <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId19"/>
     <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId20"/>
-    <sheet name="AtomTypes" sheetId="30" r:id="rId21"/>
-    <sheet name="Atom-Attributes" sheetId="31" r:id="rId22"/>
+    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId21"/>
+    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="239">
   <si>
     <t>AT-1</t>
   </si>
@@ -142,12 +142,6 @@
     <t>Element</t>
   </si>
   <si>
-    <t>BondPattern-2</t>
-  </si>
-  <si>
-    <t>BondPattern</t>
-  </si>
-  <si>
     <t>AtomType-Name</t>
   </si>
   <si>
@@ -157,30 +151,9 @@
     <t>Atom-Types</t>
   </si>
   <si>
-    <t>ElementsDisallowed</t>
-  </si>
-  <si>
-    <t>ElementsAllowed</t>
-  </si>
-  <si>
-    <t>Hybridization</t>
-  </si>
-  <si>
     <t>FormalCharge</t>
   </si>
   <si>
-    <t>Aromatic</t>
-  </si>
-  <si>
-    <t>Ring</t>
-  </si>
-  <si>
-    <t>BondOrder</t>
-  </si>
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
     <t>Force-Field Metadata</t>
   </si>
   <si>
@@ -202,9 +175,6 @@
     <t>AtomicMass</t>
   </si>
   <si>
-    <t>PatternNomenclatureStyle</t>
-  </si>
-  <si>
     <t>ATDL</t>
   </si>
   <si>
@@ -779,6 +749,30 @@
   </si>
   <si>
     <t>[epsilon_g+[(epsilon_A-epsilon_g)/(1+exp(-k_sig*(T-T_sig)))]]*[((sigma*(a*T+b))/R)^12-((sigma*(a*T+b))/R)^6]</t>
+  </si>
+  <si>
+    <t>Nomenclature</t>
+  </si>
+  <si>
+    <t>Atom</t>
+  </si>
+  <si>
+    <t>BondedAtoms</t>
+  </si>
+  <si>
+    <t>SMILES</t>
+  </si>
+  <si>
+    <t>AtomicMass-CG</t>
+  </si>
+  <si>
+    <t>AtomicSize-CG</t>
+  </si>
+  <si>
+    <t>CG-Name</t>
+  </si>
+  <si>
+    <t>CG-Chemistry</t>
   </si>
 </sst>
 </file>
@@ -795,15 +789,6 @@
     </font>
     <font>
       <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -857,6 +842,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1031,51 +1023,49 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="6" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1093,17 +1083,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1113,10 +1104,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1477,109 +1465,109 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="52" style="23" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="18.5703125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="52" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="22" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="40"/>
-    </row>
-    <row r="2" spans="1:2" s="22" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="39"/>
+    </row>
+    <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="22" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:2" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="30"/>
-    </row>
-    <row r="4" spans="1:2" s="22" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="28"/>
+    </row>
+    <row r="4" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>151</v>
+      <c r="B5" s="24" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>150</v>
+      <c r="B6" s="27" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>150</v>
+      <c r="B7" s="25" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>150</v>
+      <c r="B8" s="26" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>150</v>
+      <c r="B9" s="27" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>150</v>
+      <c r="B10" s="27" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>150</v>
+      <c r="B11" s="25" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>150</v>
+      <c r="B12" s="27" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>150</v>
+      <c r="B13" s="27" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="33" t="s">
-        <v>150</v>
+      <c r="B14" s="31" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1619,16 +1607,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -1637,10 +1625,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -1649,10 +1637,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -1661,10 +1649,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -1673,7 +1661,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -1685,32 +1673,32 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>45</v>
+      <c r="E9" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1755,19 +1743,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -1775,7 +1763,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1787,10 +1775,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -1799,10 +1787,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -1810,47 +1798,47 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>43</v>
+      <c r="A8" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>44</v>
+      <c r="A9" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>45</v>
+      <c r="A10" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,10 +1846,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,10 +1857,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,22 +1868,22 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,58 +1895,58 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>132</v>
+      <c r="A22" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,15 +1955,15 @@
       </c>
       <c r="B23">
         <f ca="1">RAND()</f>
-        <v>0.60563741713831609</v>
+        <v>0.15555781913538702</v>
       </c>
       <c r="C23">
         <f ca="1">RAND()</f>
-        <v>0.69500099022106465</v>
+        <v>0.61115053494652427</v>
       </c>
       <c r="D23">
         <f ca="1">RAND()</f>
-        <v>0.55300013629479816</v>
+        <v>0.53388845317887834</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,15 +1972,15 @@
       </c>
       <c r="B24">
         <f t="shared" ref="B24:D26" ca="1" si="0">RAND()</f>
-        <v>0.92148105950901504</v>
+        <v>0.6772056967412019</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80086898410912477</v>
+        <v>0.72446787330165718</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67708191511491655</v>
+        <v>0.15784152056260592</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2001,15 +1989,15 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59607351710131318</v>
+        <v>0.40006714507799934</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14361003978773057</v>
+        <v>0.28000163886134699</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79373759192934401</v>
+        <v>0.82624144912708497</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,15 +2006,15 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88598058307555594</v>
+        <v>0.54193151260406913</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6632580278094008</v>
+        <v>0.70516286576904563</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3330128707294544</v>
+        <v>0.15770061987817763</v>
       </c>
     </row>
   </sheetData>
@@ -2074,16 +2062,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="39" t="s">
-        <v>198</v>
+      <c r="A1" s="37" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -2092,10 +2080,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -2104,10 +2092,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -2116,10 +2104,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2128,7 +2116,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -2140,32 +2128,32 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>45</v>
+      <c r="E9" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2219,10 +2207,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2230,10 +2218,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2241,10 +2229,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2252,10 +2240,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -2263,10 +2251,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -2274,23 +2262,23 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>45</v>
+      <c r="B9" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2336,22 +2324,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2359,10 +2347,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2370,10 +2358,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2381,10 +2369,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -2392,10 +2380,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -2403,26 +2391,26 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>45</v>
+      <c r="C9" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2479,10 +2467,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2490,10 +2478,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2501,10 +2489,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2512,10 +2500,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -2523,10 +2511,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -2534,23 +2522,23 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>45</v>
+      <c r="B9" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.25">
@@ -2601,19 +2589,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2621,10 +2609,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -2632,10 +2620,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2643,10 +2631,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -2654,37 +2642,37 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>43</v>
+      <c r="A9" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>44</v>
+      <c r="A10" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>45</v>
+      <c r="A11" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2692,10 +2680,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2703,21 +2691,21 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,64 +2716,64 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B17" s="1">
         <f ca="1">RAND()</f>
-        <v>0.90380637115995177</v>
+        <v>8.3698067462312231E-2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B18" s="1">
         <f ca="1">RAND()</f>
-        <v>0.17443211608269049</v>
+        <v>0.55517216567152272</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>125</v>
+      <c r="A22" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2794,15 +2782,15 @@
       </c>
       <c r="B23">
         <f ca="1">RAND()</f>
-        <v>0.54359890423136203</v>
+        <v>0.12148763186201905</v>
       </c>
       <c r="C23">
         <f t="shared" ref="C23:D23" ca="1" si="0">RAND()</f>
-        <v>0.31977201190745619</v>
+        <v>1.2557898511870946E-2</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90106327450591128</v>
+        <v>0.31050203365376905</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2811,15 +2799,15 @@
       </c>
       <c r="B24">
         <f t="shared" ref="B24:D27" ca="1" si="1">RAND()</f>
-        <v>0.26349153758315169</v>
+        <v>0.42444396071712087</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28069111421512105</v>
+        <v>0.78641099667624448</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5862631322938228E-3</v>
+        <v>0.56075915592275993</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2828,15 +2816,15 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68771492747391971</v>
+        <v>0.15286970034864655</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33203176760479269</v>
+        <v>0.69713126155370164</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71165420727808537</v>
+        <v>2.498958850779387E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2845,15 +2833,15 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50544384446733692</v>
+        <v>0.89470238281895997</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86954046328302692</v>
+        <v>0.66960731533253504</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61878065662518222</v>
+        <v>0.57830755606751283</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2862,15 +2850,15 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95938643648415156</v>
+        <v>0.81150787602099372</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63049752865161568</v>
+        <v>0.71553854349706025</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7420914110172778E-2</v>
+        <v>0.69161184726751135</v>
       </c>
     </row>
   </sheetData>
@@ -2930,10 +2918,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2941,10 +2929,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2952,10 +2940,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2963,10 +2951,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -2974,29 +2962,29 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>45</v>
+      <c r="C8" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3051,10 +3039,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -3062,10 +3050,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -3073,10 +3061,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -3084,10 +3072,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -3095,35 +3083,35 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>45</v>
+      <c r="D8" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3180,10 +3168,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -3191,10 +3179,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -3202,10 +3190,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -3213,10 +3201,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -3224,10 +3212,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -3235,41 +3223,41 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>45</v>
+      <c r="C9" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3316,106 +3304,106 @@
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="21"/>
+    <col min="3" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="11"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>50</v>
+      <c r="A7" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="11"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="11"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3457,7 +3445,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3465,10 +3453,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -3476,10 +3464,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -3487,10 +3475,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -3498,23 +3486,23 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>45</v>
+      <c r="C7" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3547,233 +3535,142 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="32"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>231</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="str">
-        <f ca="1">CHAR(RANDBETWEEN(65,90))</f>
-        <v>X</v>
-      </c>
-      <c r="B7" s="34" t="str">
-        <f t="shared" ref="B7:E7" ca="1" si="0">CHAR(RANDBETWEEN(65,90))</f>
-        <v>H</v>
-      </c>
-      <c r="C7" s="34" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>D</v>
-      </c>
-      <c r="D7" s="34" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Z</v>
-      </c>
-      <c r="E7" s="34" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="F7" s="34">
-        <v>1</v>
-      </c>
-      <c r="G7" s="34">
-        <f ca="1">RAND()</f>
-        <v>0.17866571408185772</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="str">
-        <f t="shared" ref="A8:E11" ca="1" si="1">CHAR(RANDBETWEEN(65,90))</f>
-        <v>N</v>
-      </c>
-      <c r="B8" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>J</v>
-      </c>
-      <c r="C8" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>I</v>
-      </c>
-      <c r="D8" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>W</v>
-      </c>
-      <c r="E8" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Q</v>
-      </c>
-      <c r="F8" s="34">
-        <v>2</v>
-      </c>
-      <c r="G8" s="34">
-        <f t="shared" ref="G8:G11" ca="1" si="2">RAND()</f>
-        <v>0.8382767901284095</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>J</v>
-      </c>
-      <c r="B9" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>W</v>
-      </c>
-      <c r="C9" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>A</v>
-      </c>
-      <c r="D9" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>H</v>
-      </c>
-      <c r="E9" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="F9" s="34">
-        <v>3</v>
-      </c>
-      <c r="G9" s="34">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.21385921372533323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Y</v>
-      </c>
-      <c r="B10" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>U</v>
-      </c>
-      <c r="C10" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>M</v>
-      </c>
-      <c r="D10" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>P</v>
-      </c>
-      <c r="E10" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>N</v>
-      </c>
-      <c r="F10" s="34">
-        <v>4</v>
-      </c>
-      <c r="G10" s="34">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.10424263963205593</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>L</v>
-      </c>
-      <c r="B11" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>V</v>
-      </c>
-      <c r="C11" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>V</v>
-      </c>
-      <c r="D11" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>H</v>
-      </c>
-      <c r="E11" s="34" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>G</v>
-      </c>
-      <c r="F11" s="34">
-        <v>5</v>
-      </c>
-      <c r="G11" s="34">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.27035747172544145</v>
-      </c>
+      <c r="G6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"?, ATDL, DFF"</formula1>
+      <formula1>"?, ATDL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3786,82 +3683,114 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="17" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>33</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"?, SMILES, SMARTS, CurlySMILES, SLN, InChi"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3919,367 +3848,367 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -4307,19 +4236,19 @@
     <col min="5" max="5" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="31"/>
+    <col min="8" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -4328,14 +4257,14 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="36"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4343,14 +4272,14 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="36"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4358,14 +4287,14 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="36"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4373,14 +4302,14 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="36"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -4388,38 +4317,38 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="36"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="37"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>45</v>
+      <c r="C8" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -4466,19 +4395,19 @@
     <col min="5" max="5" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="31"/>
+    <col min="8" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -4487,14 +4416,14 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="36"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4502,14 +4431,14 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="36"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4517,14 +4446,14 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="36"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4532,14 +4461,14 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="36"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -4547,38 +4476,38 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="36"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="37"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>45</v>
+      <c r="C8" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -4624,19 +4553,19 @@
     <col min="5" max="5" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="31"/>
+    <col min="8" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -4645,14 +4574,14 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="36"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4660,14 +4589,14 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="36"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>238</v>
+        <v>162</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>228</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4675,14 +4604,14 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="36"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4690,14 +4619,14 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="36"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -4705,38 +4634,38 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="36"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="37"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>45</v>
+      <c r="C8" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -4783,28 +4712,28 @@
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="18"/>
+    <col min="10" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4812,10 +4741,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4823,10 +4752,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4834,7 +4763,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -4845,32 +4774,32 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>45</v>
+      <c r="D8" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -4917,28 +4846,28 @@
     <col min="7" max="7" width="34.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="38"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -4947,10 +4876,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -4959,10 +4888,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -4971,7 +4900,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -4983,32 +4912,32 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>45</v>
+      <c r="D8" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -5051,23 +4980,23 @@
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="18"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -5075,7 +5004,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -5086,10 +5015,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -5097,37 +5026,37 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>43</v>
+      <c r="A8" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>44</v>
+      <c r="A9" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>45</v>
+      <c r="A10" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5135,10 +5064,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5146,10 +5075,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5157,21 +5086,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5182,57 +5111,57 @@
         <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1">
         <v>456.68</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1">
         <v>6785.9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B19" s="1">
         <v>234.45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>132</v>
+      <c r="A21" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5241,15 +5170,15 @@
       </c>
       <c r="B22">
         <f ca="1">RAND()</f>
-        <v>0.42101161028852374</v>
+        <v>0.37962699363403918</v>
       </c>
       <c r="C22">
         <f t="shared" ref="C22:D22" ca="1" si="0">RAND()</f>
-        <v>0.3659579794102521</v>
+        <v>0.76823085275397329</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93701113045459672</v>
+        <v>6.7298991226545368E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5258,15 +5187,15 @@
       </c>
       <c r="B23">
         <f t="shared" ref="B23:D25" ca="1" si="1">RAND()</f>
-        <v>0.55491370368002291</v>
+        <v>0.31636509833925563</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11688447009016645</v>
+        <v>0.82373495287928877</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11587274326357877</v>
+        <v>0.39420930528539033</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5275,15 +5204,15 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4183582509953685</v>
+        <v>0.36303453254097473</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60172903059252125</v>
+        <v>0.18665259034318604</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62236140067577528</v>
+        <v>0.31017641552024144</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5292,15 +5221,15 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80951860661341946</v>
+        <v>0.68666210456261478</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14426098697680789</v>
+        <v>0.85685987139794173</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28833917211529869</v>
+        <v>0.36943394453807366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing potentials to the Excel template for CG and new corresponding Python functions.
</commit_message>
<xml_diff>
--- a/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
+++ b/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" firstSheet="14" activeTab="21"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -20,22 +20,24 @@
     <sheet name="BondPotential-FENE" sheetId="39" r:id="rId6"/>
     <sheet name="AnglePotential-Harmonic" sheetId="40" r:id="rId7"/>
     <sheet name="AnglePotential-COS2" sheetId="41" r:id="rId8"/>
-    <sheet name="AnglePotential-Tabular" sheetId="8" r:id="rId9"/>
-    <sheet name="DihedralPotential-Quadratic" sheetId="42" r:id="rId10"/>
-    <sheet name="DihedralPotential-Tabular" sheetId="11" r:id="rId11"/>
-    <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId12"/>
-    <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId13"/>
-    <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId14"/>
-    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId15"/>
-    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId16"/>
-    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId17"/>
-    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId18"/>
-    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId19"/>
-    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId20"/>
-    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId21"/>
-    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId22"/>
-    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId23"/>
-    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId24"/>
+    <sheet name="AnglePotential-Cosine" sheetId="54" r:id="rId9"/>
+    <sheet name="AnglePotential-Tabular" sheetId="8" r:id="rId10"/>
+    <sheet name="DihedralPotential-Quadratic" sheetId="42" r:id="rId11"/>
+    <sheet name="DihedralPotential-Tabular" sheetId="11" r:id="rId12"/>
+    <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId13"/>
+    <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId14"/>
+    <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId15"/>
+    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId16"/>
+    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId17"/>
+    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId18"/>
+    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId19"/>
+    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId20"/>
+    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId21"/>
+    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId22"/>
+    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId23"/>
+    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId24"/>
+    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId25"/>
+    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId26"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="242">
   <si>
     <t>AT-1</t>
   </si>
@@ -489,57 +491,12 @@
     <t>nm</t>
   </si>
   <si>
-    <t>klaw</t>
-  </si>
-  <si>
-    <t>ef</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>gdf</t>
-  </si>
-  <si>
     <t># Optional</t>
   </si>
   <si>
-    <t>xfg</t>
-  </si>
-  <si>
-    <t>sfg</t>
-  </si>
-  <si>
-    <t>srdg</t>
-  </si>
-  <si>
-    <t>bsr</t>
-  </si>
-  <si>
-    <t>rshnyk</t>
-  </si>
-  <si>
-    <t>fhdsr</t>
-  </si>
-  <si>
-    <t>fgh</t>
-  </si>
-  <si>
-    <t>jyt</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>fdsjh</t>
-  </si>
-  <si>
-    <t>fn</t>
-  </si>
-  <si>
-    <t>sth</t>
-  </si>
-  <si>
     <t>FENE</t>
   </si>
   <si>
@@ -811,6 +768,24 @@
   </si>
   <si>
     <t>c_ij-units</t>
+  </si>
+  <si>
+    <t>bond-length-units</t>
+  </si>
+  <si>
+    <t>Å</t>
+  </si>
+  <si>
+    <t>bond-length</t>
+  </si>
+  <si>
+    <t>Cosine</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Ka*[1+cos(theta)]</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1474,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1590,7 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"?, Atomistic - Class I, Atomistic - Class II, Atomistic - Bond Order, Atomistic - ReaxFF, Atomistic - Polarizable, Atomistic - United Atom (UA), Coarse-Grained (CG) - Pseudo-Atom"</formula1>
+      <formula1>"?, Atomistic - Class I, Atomistic - Class II, Atomistic - Bond Order, Atomistic - ReaxFF, Atomistic - Polarizable, Atomistic - United Atom (UA), Coarse-Grained - Pseudo-Atom"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1624,6 +1599,212 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="21" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22:E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"degrees,radians"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"Kcal/mole"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"Kcal/mole-degrees,Kcal/mole-radians"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
@@ -1655,7 +1836,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -1664,10 +1845,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -1676,10 +1857,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -1688,10 +1869,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -1700,7 +1881,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -1725,10 +1906,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>34</v>
@@ -1762,16 +1943,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="22" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,22 +2021,18 @@
       <c r="A8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="D9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,7 +2040,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1873,9 +2050,7 @@
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="D12" s="3" t="s">
         <v>120</v>
       </c>
@@ -1884,9 +2059,7 @@
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="D13" s="3" t="s">
         <v>120</v>
       </c>
@@ -1895,9 +2068,7 @@
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="D14" s="3" t="s">
         <v>120</v>
       </c>
@@ -1906,9 +2077,7 @@
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="D15" s="3" t="s">
         <v>120</v>
       </c>
@@ -1917,9 +2086,7 @@
       <c r="A16" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>120</v>
@@ -1929,9 +2096,7 @@
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>120</v>
@@ -1941,36 +2106,30 @@
       <c r="A18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1986,74 +2145,6 @@
       </c>
       <c r="D22" s="14" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <f ca="1">RAND()</f>
-        <v>0.84275317876823275</v>
-      </c>
-      <c r="C23">
-        <f ca="1">RAND()</f>
-        <v>0.95024648201982076</v>
-      </c>
-      <c r="D23">
-        <f ca="1">RAND()</f>
-        <v>0.87444534014966446</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <f t="shared" ref="B24:D26" ca="1" si="0">RAND()</f>
-        <v>0.69611285496377107</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.4232824196537872E-2</v>
-      </c>
-      <c r="D24">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.92490811921076854</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.39356219360841105</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4405433760116696</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49954199248728737</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.39516624218475793</v>
-      </c>
-      <c r="C26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.26326053195895116</v>
-      </c>
-      <c r="D26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.92753147284180637</v>
       </c>
     </row>
   </sheetData>
@@ -2079,7 +2170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
@@ -2102,7 +2193,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="37" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2110,7 +2201,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -2119,10 +2210,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -2131,10 +2222,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -2143,10 +2234,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2155,7 +2246,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -2180,10 +2271,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>34</v>
@@ -2217,7 +2308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2249,7 +2340,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2257,10 +2348,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2268,10 +2359,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2279,7 +2370,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -2290,10 +2381,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -2305,10 +2396,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>34</v>
@@ -2342,7 +2433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2378,7 +2469,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2386,10 +2477,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2397,10 +2488,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2408,7 +2499,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -2419,10 +2510,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -2437,10 +2528,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>34</v>
@@ -2477,7 +2568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2509,7 +2600,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2517,10 +2608,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2528,10 +2619,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2539,7 +2630,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -2550,10 +2641,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -2565,10 +2656,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>34</v>
@@ -2607,16 +2698,135 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"Lennard-Jones (9-6) [Class 2 Form]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"epsilon*[2*(sigma/R)^9-3*(sigma/R)^6]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"?,kcal/mol,kJ/mol,Reduced"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"?,Å,nm,Reduced"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="22" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2861,7 @@
         <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -2670,7 +2880,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>133</v>
@@ -2695,7 +2905,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2703,7 +2913,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2711,16 +2921,13 @@
         <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
-        <v>157</v>
-      </c>
       <c r="C13" s="3" t="s">
         <v>120</v>
       </c>
@@ -2729,9 +2936,6 @@
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>158</v>
-      </c>
       <c r="C14" s="3" t="s">
         <v>120</v>
       </c>
@@ -2740,9 +2944,7 @@
       <c r="A15" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
         <v>120</v>
       </c>
@@ -2751,9 +2953,7 @@
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1">
-        <v>5</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
         <v>120</v>
       </c>
@@ -2762,24 +2962,18 @@
       <c r="A17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="1">
-        <f ca="1">RAND()</f>
-        <v>5.8981097121497461E-2</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="1">
-        <f ca="1">RAND()</f>
-        <v>0.94608635377194328</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2788,7 +2982,7 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2797,7 +2991,7 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2813,91 +3007,6 @@
       </c>
       <c r="D22" s="14" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <f ca="1">RAND()</f>
-        <v>0.11034065062256981</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ref="C23:D23" ca="1" si="0">RAND()</f>
-        <v>0.31691624417485131</v>
-      </c>
-      <c r="D23">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.84634356647325082</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <f t="shared" ref="B24:D27" ca="1" si="1">RAND()</f>
-        <v>0.77244977990445418</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.84876770819082703</v>
-      </c>
-      <c r="D24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.59931273599546619</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.49639800758707142</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.27444253211616265</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.1588744238781844</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.26003230302098035</v>
-      </c>
-      <c r="C26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.65891555566211868</v>
-      </c>
-      <c r="D26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.95447459963237147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.64006522583118486</v>
-      </c>
-      <c r="C27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.26734380194719876</v>
-      </c>
-      <c r="D27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.20990238036582942</v>
       </c>
     </row>
   </sheetData>
@@ -2926,7 +3035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2960,7 +3069,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -2968,10 +3077,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -2979,10 +3088,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -2990,7 +3099,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -3008,13 +3117,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>34</v>
@@ -3039,288 +3148,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>"Weeks-Chandler-Anderson"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:C3">
-      <formula1>"Mie"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
-      <formula1>"C*epsilon*[(sigma/R)^m_rep-(sigma/R)^n_att]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5">
-      <formula1>"?, kcal/mol, kJ/mol"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6">
-      <formula1>"?, Å, nm"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:L9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C7 B6">
-      <formula1>"?, Å, nm"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5">
-      <formula1>"?, kcal/mol, kJ/mol"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
-      <formula1>"C*epsilon*[(sigma/R)^m_rep-(sigma/R)^n_att]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
-      <formula1>"Mie"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"Energy Renormalization"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"[epsilon_g+[(epsilon_A-epsilon_g)/(1+exp(-k_sig*(T-T_sig)))]]*[((sigma*(a*T+b))/R)^12-((sigma*(a*T+b))/R)^6]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>"K"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3468,6 +3295,288 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:C3">
+      <formula1>"Mie"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+      <formula1>"C*epsilon*[(sigma/R)^m_rep-(sigma/R)^n_att]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5">
+      <formula1>"?, kcal/mol, kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C7 B6">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5">
+      <formula1>"?, kcal/mol, kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+      <formula1>"C*epsilon*[(sigma/R)^m_rep-(sigma/R)^n_att]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>"Mie"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"Energy Renormalization"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"[epsilon_g+[(epsilon_A-epsilon_g)/(1+exp(-k_sig*(T-T_sig)))]]*[((sigma*(a*T+b))/R)^12-((sigma*(a*T+b))/R)^6]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>"K"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F7"/>
@@ -3484,7 +3593,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3495,7 +3604,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -3503,10 +3612,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -3514,10 +3623,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -3532,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>34</v>
@@ -3569,7 +3678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -3590,7 +3699,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3603,7 +3712,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -3611,10 +3720,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -3622,10 +3731,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -3633,10 +3742,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -3644,7 +3753,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>142</v>
@@ -3662,13 +3771,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>34</v>
@@ -3702,14 +3811,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3723,7 +3832,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3735,7 +3844,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -3743,10 +3852,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -3754,10 +3863,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -3765,7 +3874,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -3783,10 +3892,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>34</v>
@@ -3817,7 +3926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -3854,7 +3963,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>39</v>
@@ -3880,10 +3989,10 @@
         <v>28</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D6" s="39" t="s">
         <v>31</v>
@@ -3965,7 +4074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -3998,10 +4107,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4019,19 +4128,19 @@
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4551,7 +4660,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4563,10 +4672,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4578,10 +4687,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4593,7 +4702,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -4623,10 +4732,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>34</v>
@@ -4665,154 +4774,192 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="20" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C40" sqref="C40"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="29"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="34"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>236</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>163</v>
+        <v>237</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="34"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="34"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="35"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>36</v>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"Å,nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"Kcal/mole"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"?, Å, nm"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"K*(R-R0)^2"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"Harmonic"</formula1>
+      <formula1>"Kcal/mole-Å"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4868,7 +5015,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4880,10 +5027,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -4895,10 +5042,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4910,7 +5057,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>142</v>
@@ -4940,10 +5087,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>34</v>
@@ -5020,7 +5167,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -5028,10 +5175,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -5039,10 +5186,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -5050,7 +5197,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -5071,13 +5218,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>34</v>
@@ -5154,7 +5301,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -5163,10 +5310,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -5175,10 +5322,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -5187,7 +5334,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -5209,13 +5356,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>34</v>
@@ -5254,287 +5401,115 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="21" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="16"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="G7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="H7" s="15" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" s="1">
-        <v>456.68</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" s="1">
-        <v>6785.9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" s="1">
-        <v>234.45</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <f ca="1">RAND()</f>
-        <v>0.15270466157177709</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:D22" ca="1" si="0">RAND()</f>
-        <v>0.97578628631597308</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.42922116598557958</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23">
-        <f t="shared" ref="B23:D25" ca="1" si="1">RAND()</f>
-        <v>0.5585078357985408</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.75173182376744196</v>
-      </c>
-      <c r="D23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.72525513299831657</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.5016245677459239</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.22100400007537968</v>
-      </c>
-      <c r="D24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.96377859924382403</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.11767651932550049</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.80699910016809284</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.36638007876438761</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"Cosine"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>"degrees,radians"</formula1>
+      <formula1>"Ka*[1+cos(theta)]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"Kcal/mole"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"Kcal/mole-degrees,Kcal/mole-radians"</formula1>
+      <formula1>"?,kcal,Joules,Reduced"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>